<commit_message>
Removed submodule and added project files
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,90 +436,38 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Student ID</t>
+          <t>Folder Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Timestamp</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Folder Name</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>vishal kotnod_181</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2025-02-23 13:19:13</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>2025-04-25 08:01:59</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>vishal kotnod_181</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-02-23 13:20:28</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-02-23 13:29:28</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-02-23 13:35:40</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>2025-04-26 15:28:38</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>